<commit_message>
feat added for pdf
</commit_message>
<xml_diff>
--- a/src/templates/Amoladora.xlsx
+++ b/src/templates/Amoladora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tesisSanCristobal\FormsSinAuth\BackendForm\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F691E9-5192-4A31-8D04-6BB277A5A169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871AF107-05B8-43FF-A0E5-079E22F9A897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1035,8 +1035,44 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1044,110 +1080,80 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1159,97 +1165,91 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1297,63 +1297,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>507427</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>33616</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>941775</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>134469</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 83">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:srcRect l="3113" t="6974" r="54669" b="4757"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="507427" y="3597087"/>
-          <a:ext cx="3459936" cy="2420471"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>175371</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>81995</xdr:rowOff>
@@ -1378,7 +1321,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:srcRect l="4958" t="1744" b="1340"/>
         <a:stretch>
           <a:fillRect/>
@@ -1388,63 +1331,6 @@
         <a:xfrm>
           <a:off x="175371" y="11431313"/>
           <a:ext cx="3585664" cy="2551387"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>257738</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>56029</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>46140</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>168086</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 83">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-        </a:blip>
-        <a:srcRect l="46454" t="2217" r="-11253" b="-37462"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="257738" y="6936441"/>
-          <a:ext cx="3979402" cy="2779057"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1742,7 +1628,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1788,7 +1674,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02EABF7-90F4-88F6-EAE7-BBF32BED6AB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1797,7 +1683,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1832,7 +1718,7 @@
         <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E8E8DB-3157-9524-EABF-0A2F1491F318}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1841,7 +1727,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1861,22 +1747,66 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>259976</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>43018</xdr:rowOff>
+      <xdr:colOff>313764</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>338853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>838179</xdr:colOff>
+      <xdr:colOff>891967</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>344178</xdr:rowOff>
+      <xdr:rowOff>254531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D8A7D08-C40D-166E-BBC2-F4F3577383B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="313764" y="5699747"/>
+          <a:ext cx="3697921" cy="1072125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>117878</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>879699</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>29460</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64B385BC-32BD-2B81-9CE3-AFD27F06D26B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1892,8 +1822,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="259976" y="5789394"/>
-          <a:ext cx="3697921" cy="1072125"/>
+          <a:off x="268941" y="7020702"/>
+          <a:ext cx="3730476" cy="2027252"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>412375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>64432</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>851646</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25572</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35A7811C-E50A-0844-C671-5D2C0AF23D3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="412375" y="3497914"/>
+          <a:ext cx="3558989" cy="2274034"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2258,8 +2232,8 @@
   </sheetPr>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2278,57 +2252,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="76" t="s">
+      <c r="A1" s="133"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="77" t="s">
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="135" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="77"/>
+      <c r="M1" s="135"/>
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="78" t="s">
+      <c r="A2" s="133"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="78"/>
+      <c r="M2" s="136"/>
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="79"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
+      <c r="A3" s="137"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
+      <c r="M3" s="137"/>
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" s="5" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2343,17 +2317,17 @@
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="72" t="s">
+      <c r="B5" s="85"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="81"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86"/>
       <c r="H5" s="65"/>
       <c r="I5" s="29"/>
       <c r="J5" s="29"/>
@@ -2363,38 +2337,38 @@
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="72" t="s">
+      <c r="B6" s="85"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="73"/>
-      <c r="G6" s="81"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="65"/>
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
-      <c r="K6" s="80" t="s">
+      <c r="K6" s="138" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="80"/>
+      <c r="L6" s="138"/>
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="72" t="s">
+      <c r="B7" s="86"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="73"/>
-      <c r="G7" s="81"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="86"/>
       <c r="H7" s="65"/>
       <c r="I7" s="32"/>
       <c r="J7" s="32"/>
@@ -2407,19 +2381,19 @@
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="93" t="s">
+      <c r="B8" s="86"/>
+      <c r="C8" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="94"/>
-      <c r="E8" s="72" t="s">
+      <c r="D8" s="116"/>
+      <c r="E8" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="73"/>
-      <c r="G8" s="81"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="66" t="s">
         <v>28</v>
       </c>
@@ -2434,17 +2408,17 @@
       <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="72" t="s">
+      <c r="B9" s="85"/>
+      <c r="C9" s="117"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="73"/>
-      <c r="G9" s="81"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="86"/>
       <c r="H9" s="65"/>
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
@@ -2467,78 +2441,78 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:14" s="12" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="95"/>
-      <c r="B11" s="95"/>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="95"/>
-      <c r="M11" s="95"/>
+      <c r="A11" s="118"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="118"/>
     </row>
     <row r="12" spans="1:14" s="12" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71" t="s">
+      <c r="B12" s="122"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="100" t="s">
+      <c r="F12" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="101"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="99" t="s">
+      <c r="G12" s="125"/>
+      <c r="H12" s="126"/>
+      <c r="I12" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="99"/>
-      <c r="K12" s="100" t="s">
+      <c r="J12" s="123"/>
+      <c r="K12" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="101"/>
-      <c r="M12" s="102"/>
+      <c r="L12" s="125"/>
+      <c r="M12" s="126"/>
     </row>
     <row r="13" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="71"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="105"/>
+      <c r="A13" s="122"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="129"/>
       <c r="I13" s="64" t="s">
         <v>2</v>
       </c>
       <c r="J13" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="103"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="105"/>
+      <c r="K13" s="127"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="129"/>
     </row>
     <row r="14" spans="1:14" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="96"/>
-      <c r="B14" s="97"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="97"/>
-      <c r="I14" s="97"/>
-      <c r="J14" s="97"/>
-      <c r="K14" s="97"/>
-      <c r="L14" s="97"/>
-      <c r="M14" s="98"/>
+      <c r="A14" s="119"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="121"/>
     </row>
     <row r="15" spans="1:14" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="42"/>
@@ -2548,11 +2522,11 @@
       <c r="E15" s="67">
         <v>1</v>
       </c>
-      <c r="F15" s="84" t="s">
+      <c r="F15" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="85"/>
-      <c r="H15" s="86"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="143"/>
       <c r="I15" s="45"/>
       <c r="J15" s="46"/>
       <c r="K15" s="47"/>
@@ -2567,11 +2541,11 @@
       <c r="E16" s="68">
         <v>2</v>
       </c>
-      <c r="F16" s="106" t="s">
+      <c r="F16" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="107"/>
-      <c r="H16" s="108"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="132"/>
       <c r="I16" s="40"/>
       <c r="J16" s="41"/>
       <c r="K16" s="34"/>
@@ -2586,11 +2560,11 @@
       <c r="E17" s="68">
         <v>3</v>
       </c>
-      <c r="F17" s="90" t="s">
+      <c r="F17" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="91"/>
-      <c r="H17" s="92"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="82"/>
       <c r="I17" s="40"/>
       <c r="J17" s="41"/>
       <c r="K17" s="34"/>
@@ -2605,11 +2579,11 @@
       <c r="E18" s="68">
         <v>4</v>
       </c>
-      <c r="F18" s="90" t="s">
+      <c r="F18" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="91"/>
-      <c r="H18" s="92"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="82"/>
       <c r="I18" s="40"/>
       <c r="J18" s="41"/>
       <c r="K18" s="34"/>
@@ -2624,11 +2598,11 @@
       <c r="E19" s="68">
         <v>5</v>
       </c>
-      <c r="F19" s="90" t="s">
+      <c r="F19" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="91"/>
-      <c r="H19" s="92"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="82"/>
       <c r="I19" s="40"/>
       <c r="J19" s="41"/>
       <c r="K19" s="34"/>
@@ -2643,11 +2617,11 @@
       <c r="E20" s="68">
         <v>6</v>
       </c>
-      <c r="F20" s="90" t="s">
+      <c r="F20" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="91"/>
-      <c r="H20" s="92"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="82"/>
       <c r="I20" s="40"/>
       <c r="J20" s="41"/>
       <c r="K20" s="34"/>
@@ -2662,16 +2636,16 @@
       <c r="E21" s="68">
         <v>7</v>
       </c>
-      <c r="F21" s="90" t="s">
+      <c r="F21" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="91"/>
-      <c r="H21" s="92"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="82"/>
       <c r="I21" s="40"/>
       <c r="J21" s="41"/>
-      <c r="K21" s="87"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="89"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="78"/>
+      <c r="M21" s="79"/>
     </row>
     <row r="22" spans="1:13" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="50"/>
@@ -2681,16 +2655,16 @@
       <c r="E22" s="68">
         <v>8</v>
       </c>
-      <c r="F22" s="141" t="s">
+      <c r="F22" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="142"/>
-      <c r="H22" s="143"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="76"/>
       <c r="I22" s="40"/>
       <c r="J22" s="41"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="89"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
     </row>
     <row r="23" spans="1:13" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="51"/>
@@ -2700,11 +2674,11 @@
       <c r="E23" s="68">
         <v>9</v>
       </c>
-      <c r="F23" s="90" t="s">
+      <c r="F23" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="91"/>
-      <c r="H23" s="92"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="82"/>
       <c r="I23" s="40"/>
       <c r="J23" s="41"/>
       <c r="K23" s="37"/>
@@ -2719,11 +2693,11 @@
       <c r="E24" s="68">
         <v>10</v>
       </c>
-      <c r="F24" s="113" t="s">
+      <c r="F24" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="113"/>
-      <c r="H24" s="113"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
       <c r="I24" s="40"/>
       <c r="J24" s="41"/>
       <c r="K24" s="37"/>
@@ -2738,16 +2712,16 @@
       <c r="E25" s="68">
         <v>11</v>
       </c>
-      <c r="F25" s="90" t="s">
+      <c r="F25" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="91"/>
-      <c r="H25" s="92"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="82"/>
       <c r="I25" s="40"/>
       <c r="J25" s="41"/>
-      <c r="K25" s="138"/>
-      <c r="L25" s="139"/>
-      <c r="M25" s="140"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="73"/>
     </row>
     <row r="26" spans="1:13" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50"/>
@@ -2757,16 +2731,16 @@
       <c r="E26" s="68">
         <v>12</v>
       </c>
-      <c r="F26" s="90" t="s">
+      <c r="F26" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="91"/>
-      <c r="H26" s="92"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="82"/>
       <c r="I26" s="40"/>
       <c r="J26" s="41"/>
-      <c r="K26" s="138"/>
-      <c r="L26" s="139"/>
-      <c r="M26" s="140"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="73"/>
     </row>
     <row r="27" spans="1:13" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="50"/>
@@ -2776,11 +2750,11 @@
       <c r="E27" s="68">
         <v>13</v>
       </c>
-      <c r="F27" s="113" t="s">
+      <c r="F27" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="113"/>
-      <c r="H27" s="113"/>
+      <c r="G27" s="83"/>
+      <c r="H27" s="83"/>
       <c r="I27" s="40"/>
       <c r="J27" s="41"/>
       <c r="K27" s="34"/>
@@ -2795,16 +2769,16 @@
       <c r="E28" s="68">
         <v>14</v>
       </c>
-      <c r="F28" s="90" t="s">
+      <c r="F28" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="91"/>
-      <c r="H28" s="92"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="82"/>
       <c r="I28" s="40"/>
       <c r="J28" s="41"/>
-      <c r="K28" s="138"/>
-      <c r="L28" s="139"/>
-      <c r="M28" s="140"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="73"/>
     </row>
     <row r="29" spans="1:13" s="11" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="50"/>
@@ -2814,11 +2788,11 @@
       <c r="E29" s="68">
         <v>15</v>
       </c>
-      <c r="F29" s="90" t="s">
+      <c r="F29" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="G29" s="91"/>
-      <c r="H29" s="92"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="82"/>
       <c r="I29" s="40"/>
       <c r="J29" s="41"/>
       <c r="K29" s="34"/>
@@ -2833,11 +2807,11 @@
       <c r="E30" s="68">
         <v>16</v>
       </c>
-      <c r="F30" s="90" t="s">
+      <c r="F30" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="91"/>
-      <c r="H30" s="92"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="82"/>
       <c r="I30" s="40"/>
       <c r="J30" s="41"/>
       <c r="K30" s="34"/>
@@ -2852,11 +2826,11 @@
       <c r="E31" s="68">
         <v>17</v>
       </c>
-      <c r="F31" s="90" t="s">
+      <c r="F31" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="91"/>
-      <c r="H31" s="92"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="82"/>
       <c r="I31" s="40"/>
       <c r="J31" s="41"/>
       <c r="K31" s="34"/>
@@ -2871,11 +2845,11 @@
       <c r="E32" s="68">
         <v>18</v>
       </c>
-      <c r="F32" s="90" t="s">
+      <c r="F32" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="91"/>
-      <c r="H32" s="92"/>
+      <c r="G32" s="81"/>
+      <c r="H32" s="82"/>
       <c r="I32" s="40"/>
       <c r="J32" s="41"/>
       <c r="K32" s="34"/>
@@ -2883,20 +2857,20 @@
       <c r="M32" s="36"/>
     </row>
     <row r="33" spans="1:13" s="11" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="109" t="s">
+      <c r="A33" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="110"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="112"/>
+      <c r="D33" s="112"/>
       <c r="E33" s="68">
         <v>19</v>
       </c>
-      <c r="F33" s="90" t="s">
+      <c r="F33" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="91"/>
-      <c r="H33" s="92"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="82"/>
       <c r="I33" s="40"/>
       <c r="J33" s="41"/>
       <c r="K33" s="34"/>
@@ -2911,11 +2885,11 @@
       <c r="E34" s="68">
         <v>20</v>
       </c>
-      <c r="F34" s="91" t="s">
+      <c r="F34" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="91"/>
-      <c r="H34" s="92"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="82"/>
       <c r="I34" s="40"/>
       <c r="J34" s="41"/>
       <c r="K34" s="34"/>
@@ -2930,11 +2904,11 @@
       <c r="E35" s="68">
         <v>21</v>
       </c>
-      <c r="F35" s="111" t="s">
+      <c r="F35" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="111"/>
-      <c r="H35" s="112"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="114"/>
       <c r="I35" s="40"/>
       <c r="J35" s="41"/>
       <c r="K35" s="34"/>
@@ -2946,19 +2920,19 @@
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="21"/>
-      <c r="E36" s="71" t="s">
+      <c r="E36" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="71"/>
-      <c r="I36" s="71"/>
-      <c r="J36" s="71"/>
-      <c r="K36" s="71" t="s">
+      <c r="F36" s="122"/>
+      <c r="G36" s="122"/>
+      <c r="H36" s="122"/>
+      <c r="I36" s="122"/>
+      <c r="J36" s="122"/>
+      <c r="K36" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="L36" s="71"/>
-      <c r="M36" s="71"/>
+      <c r="L36" s="122"/>
+      <c r="M36" s="122"/>
     </row>
     <row r="37" spans="1:13" s="11" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="50"/>
@@ -2970,11 +2944,11 @@
       <c r="E37" s="68">
         <v>22</v>
       </c>
-      <c r="F37" s="117" t="s">
+      <c r="F37" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="117"/>
-      <c r="H37" s="118"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="91"/>
       <c r="I37" s="40"/>
       <c r="J37" s="41"/>
       <c r="K37" s="34"/>
@@ -2989,11 +2963,11 @@
       <c r="E38" s="68">
         <v>23</v>
       </c>
-      <c r="F38" s="91" t="s">
+      <c r="F38" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="91"/>
-      <c r="H38" s="92"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="82"/>
       <c r="I38" s="40"/>
       <c r="J38" s="41"/>
       <c r="K38" s="34"/>
@@ -3008,11 +2982,11 @@
       <c r="E39" s="68">
         <v>24</v>
       </c>
-      <c r="F39" s="91" t="s">
+      <c r="F39" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="91"/>
-      <c r="H39" s="92"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="82"/>
       <c r="I39" s="40"/>
       <c r="J39" s="41"/>
       <c r="K39" s="34"/>
@@ -3027,11 +3001,11 @@
       <c r="E40" s="69">
         <v>25</v>
       </c>
-      <c r="F40" s="119" t="s">
+      <c r="F40" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="G40" s="119"/>
-      <c r="H40" s="120"/>
+      <c r="G40" s="92"/>
+      <c r="H40" s="93"/>
       <c r="I40" s="59"/>
       <c r="J40" s="60"/>
       <c r="K40" s="61"/>
@@ -3039,48 +3013,48 @@
       <c r="M40" s="63"/>
     </row>
     <row r="41" spans="1:13" s="11" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="121" t="s">
+      <c r="A41" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="122"/>
-      <c r="C41" s="122"/>
-      <c r="D41" s="123"/>
-      <c r="E41" s="132" t="s">
+      <c r="B41" s="95"/>
+      <c r="C41" s="95"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="133"/>
-      <c r="G41" s="133"/>
-      <c r="H41" s="133"/>
-      <c r="I41" s="133"/>
-      <c r="J41" s="134"/>
-      <c r="K41" s="127" t="s">
+      <c r="F41" s="106"/>
+      <c r="G41" s="106"/>
+      <c r="H41" s="106"/>
+      <c r="I41" s="106"/>
+      <c r="J41" s="107"/>
+      <c r="K41" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="L41" s="127"/>
-      <c r="M41" s="128"/>
+      <c r="L41" s="100"/>
+      <c r="M41" s="101"/>
     </row>
     <row r="42" spans="1:13" s="11" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="124"/>
-      <c r="B42" s="125"/>
-      <c r="C42" s="125"/>
-      <c r="D42" s="126"/>
-      <c r="E42" s="135" t="s">
+      <c r="A42" s="97"/>
+      <c r="B42" s="98"/>
+      <c r="C42" s="98"/>
+      <c r="D42" s="99"/>
+      <c r="E42" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="136"/>
-      <c r="G42" s="136"/>
-      <c r="H42" s="136"/>
-      <c r="I42" s="136"/>
-      <c r="J42" s="137"/>
-      <c r="K42" s="129"/>
-      <c r="L42" s="129"/>
-      <c r="M42" s="130"/>
+      <c r="F42" s="109"/>
+      <c r="G42" s="109"/>
+      <c r="H42" s="109"/>
+      <c r="I42" s="109"/>
+      <c r="J42" s="110"/>
+      <c r="K42" s="102"/>
+      <c r="L42" s="102"/>
+      <c r="M42" s="103"/>
     </row>
     <row r="43" spans="1:13" s="12" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="131"/>
-      <c r="B43" s="131"/>
-      <c r="C43" s="131"/>
-      <c r="D43" s="131"/>
+      <c r="A43" s="104"/>
+      <c r="B43" s="104"/>
+      <c r="C43" s="104"/>
+      <c r="D43" s="104"/>
       <c r="E43" s="33"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -3091,78 +3065,57 @@
       <c r="M43" s="28"/>
     </row>
     <row r="44" spans="1:13" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="114" t="s">
+      <c r="A44" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="115"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="115"/>
-      <c r="E44" s="115"/>
-      <c r="F44" s="115"/>
-      <c r="G44" s="115"/>
-      <c r="H44" s="115"/>
-      <c r="I44" s="115"/>
-      <c r="J44" s="115"/>
-      <c r="K44" s="115"/>
-      <c r="L44" s="115"/>
-      <c r="M44" s="116"/>
+      <c r="B44" s="88"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="88"/>
+      <c r="E44" s="88"/>
+      <c r="F44" s="88"/>
+      <c r="G44" s="88"/>
+      <c r="H44" s="88"/>
+      <c r="I44" s="88"/>
+      <c r="J44" s="88"/>
+      <c r="K44" s="88"/>
+      <c r="L44" s="88"/>
+      <c r="M44" s="89"/>
     </row>
     <row r="45" spans="1:13" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="114" t="s">
+      <c r="A45" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="115"/>
-      <c r="C45" s="115"/>
-      <c r="D45" s="115"/>
-      <c r="E45" s="115"/>
-      <c r="F45" s="115"/>
-      <c r="G45" s="115"/>
-      <c r="H45" s="115"/>
-      <c r="I45" s="115"/>
-      <c r="J45" s="115"/>
-      <c r="K45" s="115"/>
-      <c r="L45" s="115"/>
-      <c r="M45" s="116"/>
+      <c r="B45" s="88"/>
+      <c r="C45" s="88"/>
+      <c r="D45" s="88"/>
+      <c r="E45" s="88"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="88"/>
+      <c r="H45" s="88"/>
+      <c r="I45" s="88"/>
+      <c r="J45" s="88"/>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="A45:M45"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="A41:D42"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:M44"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:K2"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="C8:D8"/>
@@ -3179,22 +3132,43 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:K2"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="A45:M45"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="A41:D42"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:M44"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="K25:M25"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.33" bottom="0.19685039370078741" header="0.55000000000000004" footer="0.31496062992125984"/>

</xml_diff>